<commit_message>
add changes to use case desc
</commit_message>
<xml_diff>
--- a/analysis-diagrams/SRExam_UseCaseDescription.xlsx
+++ b/analysis-diagrams/SRExam_UseCaseDescription.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielwidhiarto/ED/!TPA/Desktop/SR-Exam/analysis-diagrams/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielwidhiarto/ED/!TPA/Desktop/SR-Exam_Revision/analysis-diagrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE817928-5C86-CD41-9AA7-9F43DEAC99F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5500CE-3701-164A-B019-5C049EF14E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18920" activeTab="2" xr2:uid="{9D6EDBCB-6F14-4410-AF33-F420771ABC8E}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="18920" xr2:uid="{9D6EDBCB-6F14-4410-AF33-F420771ABC8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Change Password" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="72">
   <si>
     <t>Use case name</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>Change old password, to a new one</t>
-  </si>
-  <si>
-    <t>User enters old password first, then enters new password</t>
   </si>
   <si>
     <t>User</t>
@@ -133,9 +130,6 @@
     <t>Student cheated in exam</t>
   </si>
   <si>
-    <t>If student has cheated on exam, assistant can gives cheating report to specific student</t>
-  </si>
-  <si>
     <t>Exam Coordinator, Subject Development, Assistant</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
   </si>
   <si>
     <t>Whole class needed more time to complete the exam</t>
-  </si>
-  <si>
-    <t>Choose which exam transaction and input how many the time extension for the class</t>
   </si>
   <si>
     <t>Exam Transaction is ongoing</t>
@@ -190,9 +181,6 @@
   </si>
   <si>
     <t>Specific student needed to change seat</t>
-  </si>
-  <si>
-    <t>Select a specific student and choose a new empty seat to sit in.</t>
   </si>
   <si>
     <t>Selected student seat is changed
@@ -230,9 +218,6 @@
     <t>When student cannot upload the answer by themselves</t>
   </si>
   <si>
-    <t>Choose specific student and manually upload the answer</t>
-  </si>
-  <si>
     <t>Student answer sucessfully uploaded manually for the selected student</t>
   </si>
   <si>
@@ -263,9 +248,6 @@
     <t>Specific student need more time to complete the exam</t>
   </si>
   <si>
-    <t>Choose spesific student to be given the time extension</t>
-  </si>
-  <si>
     <t>Time extension is added to the exam transaction for the selected student
 Descriptive note detailing the time extension is appended to the transaction note</t>
   </si>
@@ -285,6 +267,60 @@
 4.1. System validate all field must be filled
 4.2. System validate duration time extension must not be more than 20 minutes
 4.3 System Automatically append a descriptive note in the transaction note</t>
+  </si>
+  <si>
+    <t>Related Use Case</t>
+  </si>
+  <si>
+    <t>Authentication where user needs to be logged in</t>
+  </si>
+  <si>
+    <t>1. Navigates to the exam transaction detail page
+2. Choose to show student details
+3. Choose specific Student
+4. Click button on offense column
+5. Input mark chearting data
+6. Submit mark cheating data</t>
+  </si>
+  <si>
+    <t>1.1. System display exam transaction detail page
+2.1. System show student details
+4.1. System show a pop up to give mark cheating
+6.1. System validate to upload the supporting images can only images file and can multiple upload
+6.2. System validate description must be filled
+6.3. System Automatically add a descriptive note in the transaction note
+6.4. System automatically add a report for exam transaction</t>
+  </si>
+  <si>
+    <t>6.1 If the supporting images not images file, display file extension must be images file message
+6.2 If description field not be filled, display description field must be filled message</t>
+  </si>
+  <si>
+    <t>View Student Details</t>
+  </si>
+  <si>
+    <t>View student seat map</t>
+  </si>
+  <si>
+    <t>View transaction details</t>
+  </si>
+  <si>
+    <t>The user goes to the profile page to start the process of changing their password. They need to enter their current password, the new password, and confirm the new password. The system checks to make sure all fields are completed, the current password is correct, the new password is different from the current one, and the new password matches the confirmation. If all validations are successful, the system updates the password in the database.</t>
+  </si>
+  <si>
+    <t>When a student is caught cheating during an exam, the Assistant, Exam Coordinator, or Subject Development personnel will document the incident by marking the student for cheating. They go to the exam transaction detail page, access the student's details, and click the button in the offense column for the specific student. A pop-up window appears, allowing them to upload supporting images and enter a description of the incident. The system validates the file types and ensures the description field is filled. Once submitted, the system automatically adds a descriptive note to the transaction note and generates a report for the incident.</t>
+  </si>
+  <si>
+    <t>During an ongoing exam, if the Exam Coordinator, Subject Development personnel, or Assistant needs to provide extra time for a specific student, they will navigate to the exam transaction detail page, select the student requiring the extension, and enter the details, including the reason and duration. The system checks that all required fields are filled, the reason for the extension is provided, and the additional time does not exceed 20 minutes. Upon successful validation, the system appends a descriptive note to the transaction record, documenting the time extension granted to the student.</t>
+  </si>
+  <si>
+    <t>To manually upload a student's answer, the user first selects an active exam transaction, prompting the system to display the exam transaction detail page. They then click the "Manual Upload" button for the specific student, triggering a pop-up window for the manual upload. The user uploads the student's answer and submits it. The system validates that the uploaded file is a .zip and ensures that the answer cannot be uploaded manually if the student has already finalized their answer or if the transaction is not ongoing.</t>
+  </si>
+  <si>
+    <t>The Exam Coordinator uses the exam scheduler page to assign proctoring assistants to oversee ongoing exam transactions. This involves choosing exam transactions that need proctoring, selecting available assistants, and ensuring there are no scheduling conflicts for the chosen assistants. The system employs an algorithm to allocate assistants, giving priority to those with the least cumulative workload. After confirming the allocation, the system updates the assistants' schedules and logs the transactions in their workload records.</t>
+  </si>
+  <si>
+    <t>During an ongoing exam, if the Exam Coordinator, Subject Development personnel, or Assistant identifies a problem with a student's seat, they navigate to the exam transaction detail page and access the student seat mapping. They select the affected student to reassign them to an available seat. The system ensures the new seat is vacant and requires a reason for the change. Once reassigned, the system updates the seat mapping and logs the change, including the student's details, previous and new seats, and the reason for the move.</t>
   </si>
 </sst>
 </file>
@@ -308,7 +344,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -451,11 +487,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -472,6 +547,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -491,7 +587,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -500,38 +608,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5639594C-6188-EE46-9788-277A978AE07B}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -864,114 +966,124 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="14"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3" ht="145" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="16"/>
+      <c r="B4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="32"/>
+    </row>
+    <row r="7" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="173" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="173" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="12"/>
+      <c r="C12" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="11">
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -980,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5D1158-75A2-418F-B67D-505B6893E606}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="248" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView zoomScale="250" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -997,115 +1109,125 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="14"/>
+      <c r="B1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="B2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3" ht="152" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="16"/>
+      <c r="B4" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="33"/>
+    </row>
+    <row r="7" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" ht="224" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="12"/>
+      <c r="B12" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A9:A10"/>
+  <mergeCells count="11">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1113,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C044C-D464-5544-83F2-64DB0E746D72}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="213" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="213" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,118 +1248,128 @@
     <col min="3" max="3" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="30"/>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="1:3" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
+      <c r="B11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="22"/>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="22"/>
-    </row>
-    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="22"/>
-    </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="192" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="30"/>
+      <c r="C12" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="11">
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1246,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34BE2B40-0747-9647-9A85-EFF6B1EA81E6}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="141" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1263,114 +1395,124 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="14"/>
+      <c r="B1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="9"/>
+      <c r="B2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="9"/>
+      <c r="B4" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="22"/>
+      <c r="B7" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="37"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="22"/>
-    </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="B9" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C10" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="192" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="30"/>
+      <c r="B12" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="11">
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1379,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEB4E21-39D2-7A43-9678-D50DFFC68118}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScale="210" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView topLeftCell="A4" zoomScale="210" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1392,118 +1534,128 @@
     <col min="3" max="3" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="30"/>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="1:3" ht="134" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="224" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
+      <c r="B11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
+      <c r="C11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="22"/>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="22"/>
-    </row>
-    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="22"/>
-    </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="224" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="30"/>
+      <c r="C12" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="11">
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1512,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC99C889-BF64-7943-8BB0-50C4CE0CDE19}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1525,118 +1677,128 @@
     <col min="3" max="3" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="30"/>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="25"/>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="25"/>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="35"/>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="25"/>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="21" t="s">
+      <c r="C8" s="25"/>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="21" t="s">
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
+      <c r="B11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="22"/>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="22"/>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="22"/>
-    </row>
-    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="21" t="s">
+      <c r="C11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="22"/>
-    </row>
-    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="21" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="22"/>
-    </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="176" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="30"/>
+      <c r="C12" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="11">
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>